<commit_message>
refactor(l10n): arb 파일 업데이트
</commit_message>
<xml_diff>
--- a/lib/l10n/translations.xlsx
+++ b/lib/l10n/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sangwuuyang/Documents/GitHub/DailyReceipt-Flutter/lib/l10n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA06A97D-614B-F749-B59D-BC28DC2B6626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0528E963-388F-F042-A307-15DCE6C9A97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11680" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13020" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="196">
   <si>
     <t>Key</t>
   </si>
@@ -68,6 +68,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -86,6 +87,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -104,6 +106,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -122,6 +125,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -140,6 +144,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">. </t>
     </r>
@@ -158,6 +163,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -176,6 +182,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>.</t>
     </r>
@@ -503,6 +510,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -534,6 +542,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -552,6 +561,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -570,6 +580,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">. </t>
     </r>
@@ -588,6 +599,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -606,6 +618,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>?</t>
     </r>
@@ -627,6 +640,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -722,55 +736,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Key1</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Key2</t>
-  </si>
-  <si>
-    <t>Key3</t>
-  </si>
-  <si>
-    <t>Key4</t>
-  </si>
-  <si>
-    <t>Key5</t>
-  </si>
-  <si>
-    <t>Key6</t>
-  </si>
-  <si>
-    <t>Key7</t>
-  </si>
-  <si>
-    <t>Key8</t>
-  </si>
-  <si>
-    <t>Key9</t>
-  </si>
-  <si>
-    <t>Key10</t>
-  </si>
-  <si>
-    <t>Key11</t>
-  </si>
-  <si>
-    <t>Key12</t>
-  </si>
-  <si>
-    <t>Key13</t>
-  </si>
-  <si>
-    <t>Key14</t>
-  </si>
-  <si>
-    <t>Key15</t>
-  </si>
-  <si>
-    <t>Key16</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -904,33 +869,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Key17</t>
-  </si>
-  <si>
-    <t>Key18</t>
-  </si>
-  <si>
-    <t>Key19</t>
-  </si>
-  <si>
-    <t>Key20</t>
-  </si>
-  <si>
-    <t>Key21</t>
-  </si>
-  <si>
-    <t>Key22</t>
-  </si>
-  <si>
-    <t>Key23</t>
-  </si>
-  <si>
-    <t>Key24</t>
-  </si>
-  <si>
-    <t>Key25</t>
-  </si>
-  <si>
     <t>Print Daily Receipts</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -1232,13 +1170,244 @@
   <si>
     <t>zh</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>key1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>key2</t>
+  </si>
+  <si>
+    <t>key3</t>
+  </si>
+  <si>
+    <t>key4</t>
+  </si>
+  <si>
+    <t>key5</t>
+  </si>
+  <si>
+    <t>key6</t>
+  </si>
+  <si>
+    <t>key7</t>
+  </si>
+  <si>
+    <t>key8</t>
+  </si>
+  <si>
+    <t>key9</t>
+  </si>
+  <si>
+    <t>key10</t>
+  </si>
+  <si>
+    <t>key11</t>
+  </si>
+  <si>
+    <t>key12</t>
+  </si>
+  <si>
+    <t>key13</t>
+  </si>
+  <si>
+    <t>key14</t>
+  </si>
+  <si>
+    <t>key15</t>
+  </si>
+  <si>
+    <t>key16</t>
+  </si>
+  <si>
+    <t>key17</t>
+  </si>
+  <si>
+    <t>key18</t>
+  </si>
+  <si>
+    <t>key19</t>
+  </si>
+  <si>
+    <t>key20</t>
+  </si>
+  <si>
+    <t>key21</t>
+  </si>
+  <si>
+    <t>key22</t>
+  </si>
+  <si>
+    <t>key23</t>
+  </si>
+  <si>
+    <t>key24</t>
+  </si>
+  <si>
+    <t>key25</t>
+  </si>
+  <si>
+    <t>Collect moments</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>瞬間を集める</t>
+  </si>
+  <si>
+    <r>
+      <t>收集瞬</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>间</t>
+    </r>
+  </si>
+  <si>
+    <t>Input placeholder</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>key26</t>
+  </si>
+  <si>
+    <t>Collect moments</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>No todos for this day</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectedDate</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stop</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Play</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>COPY</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>SAVE</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PIN</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Change My NickName</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logout</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delete</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ITEM COUNT</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOTAL</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Print Your Time</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>분</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>TODO</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>훌륭해요! 오늘의 집중이\n내일의 성과로 이어질 거예요.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>key27</t>
+  </si>
+  <si>
+    <t>key28</t>
+  </si>
+  <si>
+    <t>key29</t>
+  </si>
+  <si>
+    <t>key30</t>
+  </si>
+  <si>
+    <t>key31</t>
+  </si>
+  <si>
+    <t>key32</t>
+  </si>
+  <si>
+    <t>key33</t>
+  </si>
+  <si>
+    <t>key34</t>
+  </si>
+  <si>
+    <t>key35</t>
+  </si>
+  <si>
+    <t>key36</t>
+  </si>
+  <si>
+    <t>key37</t>
+  </si>
+  <si>
+    <t>key38</t>
+  </si>
+  <si>
+    <t>key39</t>
+  </si>
+  <si>
+    <t>key40</t>
+  </si>
+  <si>
+    <t>key41</t>
+  </si>
+  <si>
+    <t>key42</t>
+  </si>
+  <si>
+    <t>key43</t>
+  </si>
+  <si>
+    <t>key44</t>
+  </si>
+  <si>
+    <t>key45</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1288,6 +1457,21 @@
       <family val="2"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1309,7 +1493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1319,6 +1503,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1537,10 +1722,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
@@ -1564,513 +1749,690 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="17">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="14">
       <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
+        <v>131</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="17">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="17">
+        <v>161</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" t="s">
-        <v>69</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="17">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>9</v>
+        <v>34</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>135</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
+        <v>37</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>11</v>
+        <v>41</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17">
       <c r="A9" s="2" t="s">
-        <v>27</v>
+        <v>137</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>12</v>
+        <v>45</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>138</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>13</v>
+        <v>49</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>139</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>14</v>
+        <v>53</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17">
       <c r="A12" s="2" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>15</v>
+        <v>57</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="B13" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>19</v>
+        <v>65</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>104</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="F14" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17">
       <c r="A15" s="2" t="s">
-        <v>33</v>
+        <v>143</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="F15" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="B16" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="F16" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17">
       <c r="A17" s="2" t="s">
-        <v>35</v>
+        <v>145</v>
       </c>
       <c r="B17" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="E17" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="F17" t="s">
-        <v>117</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="17">
       <c r="A18" s="2" t="s">
-        <v>46</v>
+        <v>146</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="E18" t="s">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="F18" t="s">
-        <v>121</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17">
       <c r="A19" s="2" t="s">
-        <v>47</v>
+        <v>147</v>
       </c>
       <c r="B19" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="E19" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="F19" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17">
       <c r="A20" s="2" t="s">
-        <v>48</v>
+        <v>148</v>
       </c>
       <c r="B20" t="s">
-        <v>126</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>39</v>
+        <v>89</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="E20" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="F20" t="s">
-        <v>129</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17">
       <c r="A21" s="2" t="s">
-        <v>49</v>
+        <v>149</v>
       </c>
       <c r="B21" t="s">
-        <v>130</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>40</v>
+        <v>93</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="E21" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
       <c r="F21" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17">
       <c r="A22" s="2" t="s">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="B22" t="s">
-        <v>133</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>41</v>
+        <v>97</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="E22" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
       <c r="F22" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17">
       <c r="A23" s="2" t="s">
-        <v>51</v>
+        <v>151</v>
       </c>
       <c r="B23" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="F23" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17">
       <c r="A24" s="2" t="s">
-        <v>52</v>
+        <v>152</v>
       </c>
       <c r="B24" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="E24" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="F24" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17">
       <c r="A25" s="2" t="s">
-        <v>53</v>
+        <v>153</v>
       </c>
       <c r="B25" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="E25" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="F25" t="s">
-        <v>148</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="17">
       <c r="A26" s="2" t="s">
-        <v>54</v>
+        <v>154</v>
       </c>
       <c r="B26" t="s">
-        <v>149</v>
+        <v>112</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>151</v>
+        <v>114</v>
       </c>
       <c r="E26" t="s">
-        <v>150</v>
+        <v>113</v>
       </c>
       <c r="F26" t="s">
-        <v>152</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17">
+      <c r="A27" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B27" t="s">
+        <v>116</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17">
+      <c r="A28" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" t="s">
+        <v>121</v>
+      </c>
+      <c r="F28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17">
+      <c r="A29" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E29" t="s">
+        <v>125</v>
+      </c>
+      <c r="F29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15">
+      <c r="A30" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15">
+      <c r="A31" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15">
+      <c r="A32" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15">
+      <c r="A33" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15">
+      <c r="A34" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15">
+      <c r="A35" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15">
+      <c r="A36" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15">
+      <c r="A37" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15">
+      <c r="A38" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15">
+      <c r="A39" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15">
+      <c r="A40" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15">
+      <c r="A41" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15">
+      <c r="A42" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15">
+      <c r="A43" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15">
+      <c r="A44" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15">
+      <c r="A45" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15">
+      <c r="A46" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>